<commit_message>
module parameters a/b/dtc update
</commit_message>
<xml_diff>
--- a/ModuleParameters.xlsx
+++ b/ModuleParameters.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odysseas/Google Drive/University/Courses/EBE/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NCG\OneDrive\Documents\Utrecht University\Energy in Built\6.2 Photovoltaic (PV) systems, irradiance and PV performance evaluation\utrechtsmartdistricpartA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EEFB09B-833E-6549-82DF-0C382A61BA13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7456B-09F6-415B-859D-ACA291918AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="12540" xr2:uid="{F77A1787-10C0-4D66-87CB-783C8E3C6262}"/>
+    <workbookView xWindow="444" yWindow="132" windowWidth="22140" windowHeight="8964" xr2:uid="{F77A1787-10C0-4D66-87CB-783C8E3C6262}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -578,11 +587,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC161C11-6D82-46AE-8084-08297ACFE164}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51" style="5" bestFit="1" customWidth="1"/>
@@ -590,7 +599,7 @@
     <col min="4" max="4" width="51" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>46</v>
       </c>
@@ -604,7 +613,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -618,7 +627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -632,7 +641,7 @@
         <v>1.93</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -646,7 +655,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -660,7 +669,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
@@ -674,7 +683,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
@@ -688,7 +697,7 @@
         <v>8.5753000000000004</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
@@ -702,7 +711,7 @@
         <v>44.292099999999998</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
@@ -716,7 +725,7 @@
         <v>7.9629999999999992</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
@@ -730,7 +739,7 @@
         <v>35.0837</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
@@ -744,7 +753,7 @@
         <v>5.9999999999999995E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
@@ -758,7 +767,7 @@
         <v>-2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
@@ -772,7 +781,7 @@
         <v>0.99900000000000011</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
@@ -786,7 +795,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
@@ -800,7 +809,7 @@
         <v>-0.155</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -814,7 +823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
@@ -828,7 +837,7 @@
         <v>-0.16689999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
@@ -842,7 +851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
@@ -856,7 +865,7 @@
         <v>1.0770999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
@@ -870,7 +879,7 @@
         <v>-0.35499999999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
@@ -884,7 +893,7 @@
         <v>-13.064291000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
@@ -898,7 +907,7 @@
         <v>0.93269999999999997</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
@@ -912,7 +921,7 @@
         <v>7.2829999999999992E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
@@ -926,7 +935,7 @@
         <v>-2.402E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
@@ -940,7 +949,7 @@
         <v>3.8189999999999999E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
@@ -954,7 +963,7 @@
         <v>-2.3499999999999999E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>29</v>
       </c>
@@ -968,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>30</v>
       </c>
@@ -982,7 +991,7 @@
         <v>-6.8010000000000006E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>31</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>7.9679999999999996E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>32</v>
       </c>
@@ -1010,7 +1019,7 @@
         <v>-3.095E-5</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>33</v>
       </c>
@@ -1024,7 +1033,7 @@
         <v>4.8960000000000004E-7</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>34</v>
       </c>
@@ -1038,21 +1047,21 @@
         <v>-2.7799999999999999E-9</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="5">
-        <v>2.0299999999999998</v>
+        <v>3</v>
       </c>
       <c r="C33" s="5">
         <v>3</v>
       </c>
-      <c r="D33">
-        <v>2.58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>36</v>
       </c>
@@ -1062,39 +1071,39 @@
       <c r="C34" s="5">
         <v>1</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B35" s="5">
-        <v>-3.7488999999999999</v>
+        <v>-3.56</v>
       </c>
       <c r="C35" s="5">
         <v>-3.47</v>
       </c>
-      <c r="D35">
-        <v>-3.7566000000000002</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="5">
+        <v>-3.56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B36" s="5">
-        <v>-0.12870000000000001</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="C36" s="5">
         <v>-5.8999999999999997E-2</v>
       </c>
-      <c r="D36">
-        <v>-0.156</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="5">
+        <v>-7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>39</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>1.0049999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>40</v>
       </c>
@@ -1110,7 +1119,7 @@
         <v>-5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>41</v>
       </c>
@@ -1118,7 +1127,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>42</v>
       </c>
@@ -1126,7 +1135,7 @@
         <v>0.69</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>43</v>
       </c>
@@ -1134,7 +1143,7 @@
         <v>1.1120000000000001</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>44</v>
       </c>
@@ -1142,7 +1151,7 @@
         <v>-0.112</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>53</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>45</v>
       </c>

</xml_diff>

<commit_message>
power ac min and max values
</commit_message>
<xml_diff>
--- a/ModuleParameters.xlsx
+++ b/ModuleParameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NCG\OneDrive\Documents\Utrecht University\Energy in Built\6.2 Photovoltaic (PV) systems, irradiance and PV performance evaluation\utrechtsmartdistricpartA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fb00dc8ed84c692/Documents/Utrecht University/Energy in Built/6.2 Photovoltaic (PV) systems^J irradiance and PV performance evaluation/utrechtsmartdistricpartA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B7456B-09F6-415B-859D-ACA291918AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="13_ncr:1_{E1B7456B-09F6-415B-859D-ACA291918AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0035D4C-E9E8-416A-B59C-1627F93B2029}"/>
   <bookViews>
-    <workbookView xWindow="444" yWindow="132" windowWidth="22140" windowHeight="8964" xr2:uid="{F77A1787-10C0-4D66-87CB-783C8E3C6262}"/>
+    <workbookView minimized="1" xWindow="1812" yWindow="1812" windowWidth="17280" windowHeight="8964" xr2:uid="{F77A1787-10C0-4D66-87CB-783C8E3C6262}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC161C11-6D82-46AE-8084-08297ACFE164}">
   <dimension ref="A1:D44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>